<commit_message>
quick tests using PR map
</commit_message>
<xml_diff>
--- a/TorpedoBackend/Agent/PR_Graph.xlsx
+++ b/TorpedoBackend/Agent/PR_Graph.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <bookViews>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author/>
+    <author>Imported Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A1">
+    <comment ref="A1" authorId="0">
       <text>
-        <t xml:space="preserve">Diego Land
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Helvetica Neue"/>
+          </rPr>
+          <t>Imported Author:
+Diego Land
 	-Pedro Luis Rivera Gómez</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -27,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="361">
   <si>
     <t>Adjuntas</t>
   </si>
@@ -1115,111 +1123,184 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="6">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
-      <color rgb="FF24292E"/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="8"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <sz val="9.0"/>
-      <color rgb="FF24292E"/>
+      <sz val="9"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="9"/>
       <name val="SFMono-Regular"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF1C232"/>
-        <bgColor rgb="FFF1C232"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF93C47D"/>
-        <bgColor rgb="FF93C47D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE06666"/>
-        <bgColor rgb="FFE06666"/>
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="6">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="1" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ff24292e"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1233,10 +1314,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="4285F4"/>
@@ -1257,25 +1338,25 @@
         <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Sheets">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1284,76 +1365,66 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="129999"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="104999"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -1364,1399 +1435,2773 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </a:spPr>
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+        <a:spAutoFit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Arial"/>
+            <a:ea typeface="Arial"/>
+            <a:cs typeface="Arial"/>
+            <a:sym typeface="Arial"/>
+          </a:defRPr>
+        </a:defPPr>
+        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl1pPr>
+        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl2pPr>
+        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl3pPr>
+        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl4pPr>
+        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl5pPr>
+        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl6pPr>
+        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl7pPr>
+        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl8pPr>
+        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl9pPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="none"/>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </a:spPr>
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+        <a:noAutofit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:defPPr>
+        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl1pPr>
+        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl2pPr>
+        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl3pPr>
+        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl4pPr>
+        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl5pPr>
+        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl6pPr>
+        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl7pPr>
+        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl8pPr>
+        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl9pPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="none"/>
+      </a:style>
+    </a:lnDef>
+    <a:txDef>
+      <a:spPr>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </a:spPr>
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+        <a:spAutoFit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Arial"/>
+            <a:ea typeface="Arial"/>
+            <a:cs typeface="Arial"/>
+            <a:sym typeface="Arial"/>
+          </a:defRPr>
+        </a:defPPr>
+        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl1pPr>
+        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl2pPr>
+        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl3pPr>
+        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl4pPr>
+        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl5pPr>
+        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl6pPr>
+        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl7pPr>
+        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl8pPr>
+        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl9pPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="none"/>
+      </a:style>
+    </a:txDef>
+  </a:objectDefaults>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="37.0"/>
-    <col customWidth="1" min="2" max="2" width="8.14"/>
-    <col customWidth="1" min="3" max="3" width="47.0"/>
-    <col customWidth="1" min="4" max="4" width="25.29"/>
-    <col customWidth="1" min="5" max="5" width="27.86"/>
-    <col customWidth="1" min="6" max="6" width="26.86"/>
-    <col customWidth="1" min="7" max="7" width="25.86"/>
-    <col customWidth="1" min="8" max="8" width="26.71"/>
-    <col customWidth="1" min="9" max="9" width="26.86"/>
-    <col customWidth="1" min="10" max="10" width="28.86"/>
+    <col min="1" max="1" width="37" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.17188" style="1" customWidth="1"/>
+    <col min="3" max="3" width="47" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.8516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.8516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.8516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.6719" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.8516" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.8516" style="1" customWidth="1"/>
+    <col min="11" max="256" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="13.65" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="3">
+        <v>1.38</v>
+      </c>
+      <c r="C1" t="s" s="4">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" t="s" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" ht="14" customHeight="1">
+      <c r="A2" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="3">
+        <v>2.409259259259259</v>
+      </c>
+      <c r="C2" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s" s="4">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" ht="14" customHeight="1">
+      <c r="A3" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="3">
+        <v>2.35686274509804</v>
+      </c>
+      <c r="C3" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="C4" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s" s="4">
         <v>23</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" ht="14" customHeight="1">
+      <c r="A5" t="s" s="6">
         <v>24</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="3">
+        <v>0.4872727272727273</v>
+      </c>
+      <c r="C5" t="s" s="4">
         <v>25</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s" s="4">
         <v>26</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s" s="4">
         <v>28</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s" s="4">
         <v>29</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" ht="14" customHeight="1">
+      <c r="A6" t="s" s="6">
         <v>31</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="3">
+        <v>1.456701030927835</v>
+      </c>
+      <c r="C6" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s" s="4">
         <v>33</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s" s="4">
         <v>34</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" ht="14" customHeight="1">
+      <c r="A7" t="s" s="6">
         <v>36</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="3">
+        <v>0.9408695652173913</v>
+      </c>
+      <c r="C7" t="s" s="4">
         <v>37</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s" s="4">
         <v>38</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" t="s" s="7">
         <v>39</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="3">
+        <v>2.283157894736842</v>
+      </c>
+      <c r="C8" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="s" s="4">
         <v>41</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s" s="4">
         <v>43</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s" s="4">
         <v>44</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" ht="14" customHeight="1">
+      <c r="A9" t="s" s="6">
         <v>46</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="3">
+        <v>1.207619047619048</v>
+      </c>
+      <c r="C9" t="s" s="4">
         <v>47</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s" s="4">
         <v>48</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s" s="4">
         <v>49</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" ht="14" customHeight="1">
+      <c r="A10" t="s" s="6">
         <v>50</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="3">
+        <v>0.4605405405405406</v>
+      </c>
+      <c r="C10" t="s" s="4">
         <v>51</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s" s="4">
         <v>52</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" t="s" s="4">
         <v>53</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s" s="4">
         <v>54</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s" s="4">
         <v>55</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s" s="4">
         <v>56</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" ht="13.65" customHeight="1">
+      <c r="A11" t="s" s="7">
         <v>57</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="3">
+        <v>0.4600000000000001</v>
+      </c>
+      <c r="C11" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="s" s="4">
         <v>59</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" t="s" s="4">
         <v>60</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" t="s" s="4">
         <v>61</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" t="s" s="4">
         <v>62</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" t="s" s="4">
         <v>63</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" t="s" s="4">
         <v>64</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="s">
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" ht="14" customHeight="1">
+      <c r="A12" t="s" s="6">
         <v>65</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="3">
+        <v>1.964885496183206</v>
+      </c>
+      <c r="C12" t="s" s="4">
         <v>66</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" t="s" s="4">
         <v>67</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" t="s" s="4">
         <v>68</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" t="s" s="4">
         <v>69</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" ht="14" customHeight="1">
+      <c r="A13" t="s" s="6">
         <v>70</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s" s="4">
         <v>71</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="s" s="4">
         <v>72</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" t="s" s="4">
         <v>73</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" t="s" s="4">
         <v>74</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" t="s" s="4">
         <v>75</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" t="s" s="4">
         <v>76</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" t="s" s="4">
         <v>77</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" t="s" s="4">
         <v>78</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
+    <row r="14" ht="14" customHeight="1">
+      <c r="A14" t="s" s="6">
         <v>79</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="3">
+        <v>2.115348837209302</v>
+      </c>
+      <c r="C14" t="s" s="4">
         <v>80</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" t="s" s="4">
         <v>81</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" t="s" s="4">
         <v>82</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" t="s" s="4">
         <v>83</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" ht="14" customHeight="1">
+      <c r="A15" t="s" s="6">
         <v>84</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="3">
+        <v>0.3977142857142857</v>
+      </c>
+      <c r="C15" t="s" s="4">
         <v>85</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" t="s" s="4">
         <v>86</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" t="s" s="4">
         <v>87</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" t="s" s="4">
         <v>88</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" t="s" s="4">
         <v>89</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" ht="14" customHeight="1">
+      <c r="A16" t="s" s="6">
         <v>90</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="3">
+        <v>0.332</v>
+      </c>
+      <c r="C16" t="s" s="4">
         <v>91</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" t="s" s="4">
         <v>92</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" t="s" s="4">
         <v>93</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" t="s" s="4">
         <v>94</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" t="s" s="4">
         <v>95</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" t="s" s="4">
         <v>96</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" ht="13.65" customHeight="1">
+      <c r="A17" t="s" s="7">
         <v>97</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="3">
+        <v>0.513103448275862</v>
+      </c>
+      <c r="C17" t="s" s="4">
         <v>98</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" t="s" s="4">
         <v>99</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" t="s" s="4">
         <v>100</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" ht="14" customHeight="1">
+      <c r="A18" t="s" s="6">
         <v>101</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="3">
+        <v>0.2292307692307692</v>
+      </c>
+      <c r="C18" t="s" s="4">
         <v>102</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" t="s" s="4">
         <v>103</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" t="s" s="4">
         <v>104</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" t="s" s="4">
         <v>105</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" t="s" s="4">
         <v>106</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" t="s" s="4">
         <v>107</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" t="s" s="4">
         <v>108</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" ht="14" customHeight="1">
+      <c r="A19" t="s" s="6">
         <v>109</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="3">
+        <v>0.5721311475409836</v>
+      </c>
+      <c r="C19" t="s" s="4">
         <v>110</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" t="s" s="4">
         <v>111</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" t="s" s="4">
         <v>112</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" t="s" s="4">
         <v>113</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" t="s" s="4">
         <v>114</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" ht="14" customHeight="1">
+      <c r="A20" t="s" s="6">
         <v>115</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="3">
+        <v>1.06</v>
+      </c>
+      <c r="C20" t="s" s="4">
         <v>116</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" t="s" s="4">
         <v>117</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" t="s" s="4">
         <v>118</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" t="s" s="4">
         <v>119</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" t="s" s="4">
         <v>120</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" t="s" s="4">
         <v>121</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" t="s" s="4">
         <v>122</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" t="s" s="4">
         <v>123</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="4" t="s">
+    <row r="21" ht="14" customHeight="1">
+      <c r="A21" t="s" s="6">
         <v>124</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="3">
+        <v>0.1753846153846154</v>
+      </c>
+      <c r="C21" t="s" s="4">
         <v>125</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s" s="4">
         <v>126</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" t="s" s="4">
         <v>127</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" t="s" s="4">
         <v>128</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" t="s" s="4">
         <v>129</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="s">
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" ht="14" customHeight="1">
+      <c r="A22" t="s" s="6">
         <v>130</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="3">
+        <v>0.6818181818181818</v>
+      </c>
+      <c r="C22" t="s" s="4">
         <v>131</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" t="s" s="4">
         <v>132</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" t="s" s="4">
         <v>133</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" t="s" s="4">
         <v>134</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" t="s" s="4">
         <v>135</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" t="s" s="4">
         <v>136</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" t="s" s="4">
         <v>137</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" ht="13.65" customHeight="1">
+      <c r="A23" t="s" s="7">
         <v>138</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="3">
+        <v>0.2830769230769231</v>
+      </c>
+      <c r="C23" t="s" s="4">
         <v>139</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" t="s" s="4">
         <v>140</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" t="s" s="4">
         <v>141</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" t="s" s="4">
         <v>142</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" t="s" s="4">
         <v>143</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" t="s" s="4">
         <v>144</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="s">
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" ht="14" customHeight="1">
+      <c r="A24" t="s" s="6">
         <v>145</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="3">
+        <v>0.6260869565217392</v>
+      </c>
+      <c r="C24" t="s" s="4">
         <v>146</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" t="s" s="4">
         <v>147</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" t="s" s="4">
         <v>148</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" t="s" s="4">
         <v>149</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" t="s" s="4">
         <v>150</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" t="s" s="4">
         <v>151</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="s">
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" ht="14" customHeight="1">
+      <c r="A25" t="s" s="6">
         <v>152</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="3">
+        <v>1.20379746835443</v>
+      </c>
+      <c r="C25" t="s" s="4">
         <v>153</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" t="s" s="4">
         <v>154</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="s">
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" ht="14" customHeight="1">
+      <c r="A26" t="s" s="6">
         <v>155</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="3">
+        <v>0.728421052631579</v>
+      </c>
+      <c r="C26" t="s" s="4">
         <v>156</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" t="s" s="4">
         <v>157</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" t="s" s="4">
         <v>158</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="4" t="s">
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" ht="14" customHeight="1">
+      <c r="A27" t="s" s="6">
         <v>159</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="3" t="s">
+      <c r="B27" s="3">
+        <v>0.6389189189189189</v>
+      </c>
+      <c r="C27" t="s" s="4">
         <v>160</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" t="s" s="4">
         <v>161</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="4" t="s">
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" ht="14" customHeight="1">
+      <c r="A28" t="s" s="6">
         <v>162</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="3">
+        <v>1.32952380952381</v>
+      </c>
+      <c r="C28" t="s" s="4">
         <v>163</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" t="s" s="4">
         <v>164</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" t="s" s="4">
         <v>165</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" ht="13.65" customHeight="1">
+      <c r="A29" t="s" s="7">
         <v>166</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="3">
+        <v>0.8519999999999999</v>
+      </c>
+      <c r="C29" t="s" s="4">
         <v>167</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" t="s" s="4">
         <v>168</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="4" t="s">
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" ht="14" customHeight="1">
+      <c r="A30" t="s" s="6">
         <v>169</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="3" t="s">
+      <c r="B30" s="3">
+        <v>1.408641975308642</v>
+      </c>
+      <c r="C30" t="s" s="4">
         <v>170</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" t="s" s="4">
         <v>171</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="4" t="s">
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" ht="14" customHeight="1">
+      <c r="A31" t="s" s="6">
         <v>172</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="3" t="s">
+      <c r="B31" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="C31" t="s" s="4">
         <v>173</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" t="s" s="4">
         <v>174</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" t="s" s="4">
         <v>175</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="4" t="s">
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" ht="14" customHeight="1">
+      <c r="A32" t="s" s="6">
         <v>176</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C32" t="s" s="4">
         <v>177</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" t="s" s="4">
         <v>178</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" t="s" s="4">
         <v>179</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="4" t="s">
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" ht="14" customHeight="1">
+      <c r="A33" t="s" s="6">
         <v>180</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="3" t="s">
+      <c r="B33" s="3">
+        <v>1.577943925233645</v>
+      </c>
+      <c r="C33" t="s" s="4">
         <v>181</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" t="s" s="4">
         <v>182</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" t="s" s="4">
         <v>183</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="4" t="s">
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" ht="14" customHeight="1">
+      <c r="A34" t="s" s="6">
         <v>184</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="3" t="s">
+      <c r="B34" s="3">
+        <v>2.143298969072165</v>
+      </c>
+      <c r="C34" t="s" s="4">
         <v>185</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" t="s" s="4">
         <v>186</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="4" t="s">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" ht="14" customHeight="1">
+      <c r="A35" t="s" s="6">
         <v>187</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="3" t="s">
+      <c r="B35" s="3">
+        <v>1.96416</v>
+      </c>
+      <c r="C35" t="s" s="4">
         <v>188</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" t="s" s="4">
         <v>189</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" t="s" s="4">
         <v>190</v>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="4" t="s">
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" ht="14" customHeight="1">
+      <c r="A36" t="s" s="6">
         <v>191</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="3" t="s">
+      <c r="B36" s="3">
+        <v>0.3264</v>
+      </c>
+      <c r="C36" t="s" s="4">
         <v>192</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" t="s" s="4">
         <v>193</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" t="s" s="4">
         <v>194</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="4" t="s">
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" ht="14" customHeight="1">
+      <c r="A37" t="s" s="6">
         <v>195</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="3" t="s">
+      <c r="B37" s="3">
+        <v>2.545098039215687</v>
+      </c>
+      <c r="C37" t="s" s="4">
         <v>196</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" t="s" s="4">
         <v>197</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="4" t="s">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" ht="14" customHeight="1">
+      <c r="A38" t="s" s="6">
         <v>198</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="3" t="s">
+      <c r="B38" s="3">
+        <v>1.952903225806452</v>
+      </c>
+      <c r="C38" t="s" s="4">
         <v>199</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" t="s" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="4" t="s">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" ht="14" customHeight="1">
+      <c r="A39" t="s" s="6">
         <v>201</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="3" t="s">
+      <c r="B39" s="3">
+        <v>0.9054545454545454</v>
+      </c>
+      <c r="C39" t="s" s="4">
         <v>202</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" t="s" s="4">
         <v>203</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" t="s" s="4">
         <v>204</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" t="s" s="4">
         <v>205</v>
       </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="4" t="s">
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" ht="14" customHeight="1">
+      <c r="A40" t="s" s="6">
         <v>206</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="3" t="s">
+      <c r="B40" s="3">
+        <v>0.155</v>
+      </c>
+      <c r="C40" t="s" s="4">
         <v>207</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" t="s" s="4">
         <v>208</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" t="s" s="4">
         <v>209</v>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="4" t="s">
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" ht="14" customHeight="1">
+      <c r="A41" t="s" s="6">
         <v>210</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="3" t="s">
+      <c r="B41" s="3">
+        <v>1.832203389830509</v>
+      </c>
+      <c r="C41" t="s" s="4">
         <v>211</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" t="s" s="4">
         <v>212</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="4" t="s">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" ht="14" customHeight="1">
+      <c r="A42" t="s" s="6">
         <v>213</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="3" t="s">
+      <c r="B42" s="3">
+        <v>1.782666666666667</v>
+      </c>
+      <c r="C42" t="s" s="4">
         <v>214</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" t="s" s="4">
         <v>215</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" t="s" s="4">
         <v>216</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" t="s" s="4">
         <v>217</v>
       </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="4" t="s">
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" ht="14" customHeight="1">
+      <c r="A43" t="s" s="6">
         <v>218</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="3" t="s">
+      <c r="B43" s="3">
+        <v>2.264835164835165</v>
+      </c>
+      <c r="C43" t="s" s="4">
         <v>219</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" t="s" s="4">
         <v>220</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" t="s" s="4">
         <v>221</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" t="s" s="4">
         <v>222</v>
       </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="4" t="s">
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" ht="14" customHeight="1">
+      <c r="A44" t="s" s="6">
         <v>223</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="3" t="s">
+      <c r="B44" s="3">
+        <v>0.2497297297297297</v>
+      </c>
+      <c r="C44" t="s" s="4">
         <v>224</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" t="s" s="4">
         <v>225</v>
       </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" ht="13.65" customHeight="1">
+      <c r="A45" t="s" s="7">
         <v>226</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="3" t="s">
+      <c r="B45" s="3">
+        <v>0.4973913043478261</v>
+      </c>
+      <c r="C45" t="s" s="4">
         <v>227</v>
       </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="4" t="s">
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" ht="14" customHeight="1">
+      <c r="A46" t="s" s="6">
         <v>228</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="3" t="s">
+      <c r="B46" s="3">
+        <v>0.6368421052631579</v>
+      </c>
+      <c r="C46" t="s" s="4">
         <v>229</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" t="s" s="4">
         <v>230</v>
       </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="4" t="s">
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" ht="14" customHeight="1">
+      <c r="A47" t="s" s="6">
         <v>231</v>
       </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="3" t="s">
+      <c r="B47" s="3">
+        <v>1.114246575342466</v>
+      </c>
+      <c r="C47" t="s" s="4">
         <v>232</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" t="s" s="4">
         <v>233</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" t="s" s="4">
         <v>234</v>
       </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="4" t="s">
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" ht="14" customHeight="1">
+      <c r="A48" t="s" s="6">
         <v>235</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="3" t="s">
+      <c r="B48" s="3">
+        <v>2.069430894308943</v>
+      </c>
+      <c r="C48" t="s" s="4">
         <v>236</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" t="s" s="4">
         <v>237</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" t="s" s="4">
         <v>238</v>
       </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="4" t="s">
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" ht="14" customHeight="1">
+      <c r="A49" t="s" s="6">
         <v>239</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="3" t="s">
+      <c r="B49" s="3">
+        <v>0.6210810810810811</v>
+      </c>
+      <c r="C49" t="s" s="4">
         <v>240</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" t="s" s="4">
         <v>241</v>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="8" t="s">
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" ht="13.65" customHeight="1">
+      <c r="A50" t="s" s="7">
         <v>242</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="3" t="s">
+      <c r="B50" s="3">
+        <v>2.078823529411765</v>
+      </c>
+      <c r="C50" t="s" s="4">
         <v>243</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" t="s" s="4">
         <v>244</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" t="s" s="4">
         <v>245</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F50" t="s" s="4">
         <v>246</v>
       </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="4" t="s">
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" ht="14" customHeight="1">
+      <c r="A51" t="s" s="6">
         <v>247</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="3" t="s">
+      <c r="B51" s="3">
+        <v>2.225806451612903</v>
+      </c>
+      <c r="C51" t="s" s="4">
         <v>248</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" t="s" s="4">
         <v>249</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="4" t="s">
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" ht="14" customHeight="1">
+      <c r="A52" t="s" s="6">
         <v>250</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="3" t="s">
+      <c r="B52" s="3">
+        <v>0.9137254901960784</v>
+      </c>
+      <c r="C52" t="s" s="4">
         <v>251</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" t="s" s="4">
         <v>252</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" t="s" s="4">
         <v>253</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" t="s" s="4">
         <v>254</v>
       </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="4" t="s">
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" ht="14" customHeight="1">
+      <c r="A53" t="s" s="6">
         <v>255</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="3" t="s">
+      <c r="B53" s="3">
+        <v>0.4255999999999999</v>
+      </c>
+      <c r="C53" t="s" s="4">
         <v>256</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" t="s" s="4">
         <v>257</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" t="s" s="4">
         <v>258</v>
       </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="4" t="s">
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" ht="14" customHeight="1">
+      <c r="A54" t="s" s="6">
         <v>259</v>
       </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="3" t="s">
+      <c r="B54" s="3">
+        <v>0.4885714285714285</v>
+      </c>
+      <c r="C54" t="s" s="4">
         <v>260</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" t="s" s="4">
         <v>261</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" t="s" s="4">
         <v>262</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="F54" t="s" s="4">
         <v>263</v>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="4" t="s">
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" ht="14" customHeight="1">
+      <c r="A55" t="s" s="6">
         <v>264</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="3" t="s">
+      <c r="B55" s="3">
+        <v>0.8323809523809523</v>
+      </c>
+      <c r="C55" t="s" s="4">
         <v>265</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" t="s" s="4">
         <v>266</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" t="s" s="4">
         <v>267</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F55" t="s" s="4">
         <v>268</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="G55" t="s" s="4">
         <v>269</v>
       </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="4" t="s">
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" ht="14" customHeight="1">
+      <c r="A56" t="s" s="6">
         <v>270</v>
       </c>
-      <c r="B56" s="10"/>
-      <c r="C56" s="3" t="s">
+      <c r="B56" s="3">
+        <v>1.010434782608696</v>
+      </c>
+      <c r="C56" t="s" s="4">
         <v>271</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" t="s" s="4">
         <v>272</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" t="s" s="4">
         <v>273</v>
       </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="4" t="s">
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" ht="14" customHeight="1">
+      <c r="A57" t="s" s="6">
         <v>274</v>
       </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="3" t="s">
+      <c r="B57" s="3">
+        <v>1.293529411764706</v>
+      </c>
+      <c r="C57" t="s" s="4">
         <v>275</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" t="s" s="4">
         <v>276</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" t="s" s="4">
         <v>277</v>
       </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="4" t="s">
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" ht="14" customHeight="1">
+      <c r="A58" t="s" s="6">
         <v>278</v>
       </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="3" t="s">
+      <c r="B58" s="3">
+        <v>1.054385964912281</v>
+      </c>
+      <c r="C58" t="s" s="4">
         <v>279</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" t="s" s="4">
         <v>280</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" t="s" s="4">
         <v>281</v>
       </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="4" t="s">
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" ht="14" customHeight="1">
+      <c r="A59" t="s" s="6">
         <v>282</v>
       </c>
-      <c r="B59" s="10"/>
-      <c r="C59" s="3" t="s">
+      <c r="B59" s="3">
+        <v>2.391428571428571</v>
+      </c>
+      <c r="C59" t="s" s="4">
         <v>283</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" t="s" s="4">
         <v>284</v>
       </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="s">
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" ht="13.65" customHeight="1">
+      <c r="A60" t="s" s="7">
         <v>285</v>
       </c>
-      <c r="B60" s="10"/>
-      <c r="C60" s="3" t="s">
+      <c r="B60" s="3">
+        <v>2.515384615384616</v>
+      </c>
+      <c r="C60" t="s" s="4">
         <v>286</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" t="s" s="4">
         <v>287</v>
       </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="s">
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" ht="13.65" customHeight="1">
+      <c r="A61" t="s" s="7">
         <v>288</v>
       </c>
-      <c r="B61" s="10"/>
-      <c r="C61" s="3" t="s">
+      <c r="B61" s="3">
+        <v>0.4869565217391305</v>
+      </c>
+      <c r="C61" t="s" s="4">
         <v>289</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" t="s" s="4">
         <v>290</v>
       </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="4" t="s">
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" ht="14" customHeight="1">
+      <c r="A62" t="s" s="6">
         <v>291</v>
       </c>
-      <c r="B62" s="10"/>
-      <c r="C62" s="3" t="s">
+      <c r="B62" s="3">
+        <v>1.689902912621359</v>
+      </c>
+      <c r="C62" t="s" s="4">
         <v>292</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" t="s" s="4">
         <v>293</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" t="s" s="4">
         <v>294</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F62" t="s" s="4">
         <v>295</v>
       </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="4" t="s">
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" ht="14" customHeight="1">
+      <c r="A63" t="s" s="6">
         <v>296</v>
       </c>
-      <c r="B63" s="10"/>
-      <c r="C63" s="3" t="s">
+      <c r="B63" s="3">
+        <v>0.6381818181818182</v>
+      </c>
+      <c r="C63" t="s" s="4">
         <v>297</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" t="s" s="4">
         <v>298</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" t="s" s="4">
         <v>299</v>
       </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="4" t="s">
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" ht="14" customHeight="1">
+      <c r="A64" t="s" s="6">
         <v>300</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="3" t="s">
+      <c r="B64" s="3">
+        <v>1.812280701754386</v>
+      </c>
+      <c r="C64" t="s" s="4">
         <v>301</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" t="s" s="4">
         <v>302</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" t="s" s="4">
         <v>303</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F64" t="s" s="4">
         <v>304</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G64" t="s" s="4">
         <v>305</v>
       </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="4" t="s">
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" ht="14" customHeight="1">
+      <c r="A65" t="s" s="6">
         <v>306</v>
       </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="3" t="s">
+      <c r="B65" s="3">
+        <v>0.4454545454545454</v>
+      </c>
+      <c r="C65" t="s" s="4">
         <v>307</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" t="s" s="4">
         <v>308</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" t="s" s="4">
         <v>309</v>
       </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="4" t="s">
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" ht="14" customHeight="1">
+      <c r="A66" t="s" s="6">
         <v>310</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="3" t="s">
+      <c r="B66" s="3">
+        <v>0.1363636363636364</v>
+      </c>
+      <c r="C66" t="s" s="4">
         <v>311</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" t="s" s="4">
         <v>312</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" t="s" s="4">
         <v>313</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="F66" t="s" s="4">
         <v>314</v>
       </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="4" t="s">
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" ht="14" customHeight="1">
+      <c r="A67" t="s" s="6">
         <v>315</v>
       </c>
-      <c r="B67" s="10"/>
-      <c r="C67" s="3" t="s">
+      <c r="B67" s="3">
+        <v>2.001904761904762</v>
+      </c>
+      <c r="C67" t="s" s="4">
         <v>316</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" t="s" s="4">
         <v>317</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" t="s" s="4">
         <v>318</v>
       </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="4" t="s">
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" ht="14" customHeight="1">
+      <c r="A68" t="s" s="6">
         <v>319</v>
       </c>
-      <c r="B68" s="10"/>
-      <c r="C68" s="3" t="s">
+      <c r="B68" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="C68" t="s" s="4">
         <v>320</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" t="s" s="4">
         <v>321</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" t="s" s="4">
         <v>322</v>
       </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="4" t="s">
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" ht="14" customHeight="1">
+      <c r="A69" t="s" s="6">
         <v>323</v>
       </c>
-      <c r="B69" s="10"/>
-      <c r="C69" s="3" t="s">
+      <c r="B69" s="3">
+        <v>0.5937931034482758</v>
+      </c>
+      <c r="C69" t="s" s="4">
         <v>324</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" t="s" s="4">
         <v>325</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E69" t="s" s="4">
         <v>326</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="F69" t="s" s="4">
         <v>327</v>
       </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="4" t="s">
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" ht="14" customHeight="1">
+      <c r="A70" t="s" s="6">
         <v>328</v>
       </c>
-      <c r="B70" s="10"/>
-      <c r="C70" s="3" t="s">
+      <c r="B70" s="3">
+        <v>0.6820000000000001</v>
+      </c>
+      <c r="C70" t="s" s="4">
         <v>329</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" t="s" s="4">
         <v>330</v>
       </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="4" t="s">
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" ht="14" customHeight="1">
+      <c r="A71" t="s" s="6">
         <v>331</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="3" t="s">
+      <c r="B71" s="3">
+        <v>0.2072727272727273</v>
+      </c>
+      <c r="C71" t="s" s="4">
         <v>332</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" t="s" s="4">
         <v>333</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" t="s" s="4">
         <v>334</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="F71" t="s" s="4">
         <v>335</v>
       </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="4" t="s">
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" ht="14" customHeight="1">
+      <c r="A72" t="s" s="6">
         <v>336</v>
       </c>
-      <c r="B72" s="10"/>
-      <c r="C72" s="3" t="s">
+      <c r="B72" s="3">
+        <v>2.281408450704226</v>
+      </c>
+      <c r="C72" t="s" s="4">
         <v>337</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" t="s" s="4">
         <v>338</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E72" t="s" s="4">
         <v>339</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="F72" t="s" s="4">
         <v>340</v>
       </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="4" t="s">
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" ht="14" customHeight="1">
+      <c r="A73" t="s" s="6">
         <v>341</v>
       </c>
-      <c r="B73" s="10"/>
-      <c r="C73" s="3" t="s">
+      <c r="B73" s="3">
+        <v>0.8795918367346939</v>
+      </c>
+      <c r="C73" t="s" s="4">
         <v>342</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D73" t="s" s="4">
         <v>343</v>
       </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="4" t="s">
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+    </row>
+    <row r="74" ht="14" customHeight="1">
+      <c r="A74" t="s" s="6">
         <v>344</v>
       </c>
-      <c r="B74" s="10"/>
-      <c r="C74" s="3" t="s">
+      <c r="B74" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="C74" t="s" s="4">
         <v>345</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D74" t="s" s="4">
         <v>346</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E74" t="s" s="4">
         <v>347</v>
       </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="4" t="s">
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" ht="14" customHeight="1">
+      <c r="A75" t="s" s="6">
         <v>348</v>
       </c>
-      <c r="B75" s="10"/>
-      <c r="C75" s="3" t="s">
+      <c r="B75" s="3">
+        <v>1.069190600522193</v>
+      </c>
+      <c r="C75" t="s" s="4">
         <v>349</v>
       </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="4" t="s">
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" ht="14" customHeight="1">
+      <c r="A76" t="s" s="6">
         <v>350</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="3" t="s">
+      <c r="B76" s="3">
+        <v>0.9657142857142856</v>
+      </c>
+      <c r="C76" t="s" s="4">
         <v>351</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D76" t="s" s="4">
         <v>352</v>
       </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="4" t="s">
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+    </row>
+    <row r="77" ht="14" customHeight="1">
+      <c r="A77" t="s" s="6">
         <v>353</v>
       </c>
-      <c r="B77" s="10"/>
-      <c r="C77" s="3" t="s">
+      <c r="B77" s="3">
+        <v>0.5126984126984127</v>
+      </c>
+      <c r="C77" t="s" s="4">
         <v>354</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D77" t="s" s="4">
         <v>355</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E77" t="s" s="4">
         <v>356</v>
       </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="4" t="s">
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+    </row>
+    <row r="78" ht="14" customHeight="1">
+      <c r="A78" t="s" s="8">
         <v>357</v>
       </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="3" t="s">
+      <c r="B78" s="3">
+        <v>1.485957446808511</v>
+      </c>
+      <c r="C78" t="s" s="4">
         <v>358</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D78" t="s" s="4">
         <v>359</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E78" t="s" s="4">
         <v>360</v>
       </c>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to avoid merge errors.
</commit_message>
<xml_diff>
--- a/TorpedoBackend/Agent/PR_Graph.xlsx
+++ b/TorpedoBackend/Agent/PR_Graph.xlsx
@@ -1,25 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oatorresdiaz/Documents/Torpedo/TorpedoBackend/Agent/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF11268B-14DC-F744-9B2B-E7EE30670968}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="5880" yWindow="460" windowWidth="15960" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author/>
+    <author>Imported Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A1">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
-        <t xml:space="preserve">Diego Land
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Helvetica Neue"/>
+            <family val="2"/>
+          </rPr>
+          <t>Imported Author:
+Diego Land
 	-Pedro Luis Rivera Gómez</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -1115,115 +1133,214 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
-      <color rgb="FF24292E"/>
+      <sz val="9"/>
+      <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
-    <font/>
     <font>
-      <sz val="9.0"/>
-      <color rgb="FF24292E"/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="9"/>
       <name val="SFMono-Regular"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF1C232"/>
-        <bgColor rgb="FFF1C232"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF93C47D"/>
-        <bgColor rgb="FF93C47D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE06666"/>
-        <bgColor rgb="FFE06666"/>
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="5">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FF24292E"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1233,10 +1350,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="4285F4"/>
@@ -1257,25 +1374,25 @@
         <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Sheets">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1284,76 +1401,66 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="129999"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="104999"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -1364,85 +1471,980 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </a:spPr>
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+        <a:spAutoFit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Arial"/>
+            <a:ea typeface="Arial"/>
+            <a:cs typeface="Arial"/>
+            <a:sym typeface="Arial"/>
+          </a:defRPr>
+        </a:defPPr>
+        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl1pPr>
+        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl2pPr>
+        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl3pPr>
+        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl4pPr>
+        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl5pPr>
+        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl6pPr>
+        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl7pPr>
+        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl8pPr>
+        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl9pPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="none"/>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </a:spPr>
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+        <a:noAutofit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:defPPr>
+        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl1pPr>
+        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl2pPr>
+        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl3pPr>
+        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl4pPr>
+        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl5pPr>
+        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl6pPr>
+        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl7pPr>
+        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl8pPr>
+        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl9pPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="none"/>
+      </a:style>
+    </a:lnDef>
+    <a:txDef>
+      <a:spPr>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </a:spPr>
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+        <a:spAutoFit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Arial"/>
+            <a:ea typeface="Arial"/>
+            <a:cs typeface="Arial"/>
+            <a:sym typeface="Arial"/>
+          </a:defRPr>
+        </a:defPPr>
+        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl1pPr>
+        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl2pPr>
+        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl3pPr>
+        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl4pPr>
+        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl5pPr>
+        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl6pPr>
+        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl7pPr>
+        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl8pPr>
+        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl9pPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="none"/>
+      </a:style>
+    </a:txDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:IV78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:C82"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="37.0"/>
-    <col customWidth="1" min="2" max="2" width="8.14"/>
-    <col customWidth="1" min="3" max="3" width="47.0"/>
-    <col customWidth="1" min="4" max="4" width="25.29"/>
-    <col customWidth="1" min="5" max="5" width="27.86"/>
-    <col customWidth="1" min="6" max="6" width="26.86"/>
-    <col customWidth="1" min="7" max="7" width="25.86"/>
-    <col customWidth="1" min="8" max="8" width="26.71"/>
-    <col customWidth="1" min="9" max="9" width="26.86"/>
-    <col customWidth="1" min="10" max="10" width="28.86"/>
+    <col min="1" max="1" width="37" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="9"/>
+    <col min="3" max="3" width="47" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.83203125" style="1" customWidth="1"/>
+    <col min="11" max="256" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="13.75" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="8">
+        <v>1.2825000000000002</v>
+      </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1464,12 +2466,15 @@
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" ht="14" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="8">
+        <v>0.29833333333333328</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1482,12 +2487,18 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="14" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1497,12 +2508,19 @@
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="13.75" customHeight="1">
+      <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="8">
+        <v>2.2206849315068498</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1521,12 +2539,16 @@
       <c r="H4" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="14" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="8">
+        <v>1.7551401869158882</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1545,12 +2567,16 @@
       <c r="H5" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" ht="14" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="8">
+        <v>1.1489361702127661</v>
+      </c>
       <c r="C6" s="3" t="s">
         <v>32</v>
       </c>
@@ -1563,24 +2589,38 @@
       <c r="F6" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" ht="14" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="8">
+        <v>1.963308270676692</v>
+      </c>
       <c r="C7" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" ht="13.75" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="8">
+        <v>0.15090909090909091</v>
+      </c>
       <c r="C8" s="3" t="s">
         <v>40</v>
       </c>
@@ -1599,12 +2639,16 @@
       <c r="H8" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="14" customHeight="1">
+      <c r="A9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="8">
+        <v>2.1639655172413796</v>
+      </c>
       <c r="C9" s="3" t="s">
         <v>47</v>
       </c>
@@ -1614,12 +2658,19 @@
       <c r="E9" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="14" customHeight="1">
+      <c r="A10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="8">
+        <v>1.7889908256880735</v>
+      </c>
       <c r="C10" s="3" t="s">
         <v>51</v>
       </c>
@@ -1638,12 +2689,16 @@
       <c r="H10" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="13.75" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="8">
+        <v>2.6306250000000002</v>
+      </c>
       <c r="C11" s="3" t="s">
         <v>58</v>
       </c>
@@ -1665,12 +2720,15 @@
       <c r="I11" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="s">
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" ht="14" customHeight="1">
+      <c r="A12" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="8">
+        <v>0.19272727272727272</v>
+      </c>
       <c r="C12" s="3" t="s">
         <v>66</v>
       </c>
@@ -1683,12 +2741,18 @@
       <c r="F12" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" ht="14" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="8">
+        <v>2.227555555555556</v>
+      </c>
       <c r="C13" s="3" t="s">
         <v>71</v>
       </c>
@@ -1714,11 +2778,13 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:10" ht="14" customHeight="1">
+      <c r="A14" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="8">
+        <v>1.0656000000000001</v>
+      </c>
       <c r="C14" s="3" t="s">
         <v>80</v>
       </c>
@@ -1731,12 +2797,18 @@
       <c r="F14" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="14" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="8">
+        <v>2.7567073170731713</v>
+      </c>
       <c r="C15" s="3" t="s">
         <v>85</v>
       </c>
@@ -1752,12 +2824,17 @@
       <c r="G15" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="14" customHeight="1">
+      <c r="A16" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="8">
+        <v>2.7859756097560977</v>
+      </c>
       <c r="C16" s="3" t="s">
         <v>91</v>
       </c>
@@ -1776,12 +2853,16 @@
       <c r="H16" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" ht="13.75" customHeight="1">
+      <c r="A17" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="8">
+        <v>2.6924050632911394</v>
+      </c>
       <c r="C17" s="3" t="s">
         <v>98</v>
       </c>
@@ -1791,12 +2872,19 @@
       <c r="E17" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" ht="14" customHeight="1">
+      <c r="A18" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="8">
+        <v>1.9854098360655739</v>
+      </c>
       <c r="C18" s="3" t="s">
         <v>102</v>
       </c>
@@ -1818,12 +2906,15 @@
       <c r="I18" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" ht="14" customHeight="1">
+      <c r="A19" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="8">
+        <v>2.9061052631578947</v>
+      </c>
       <c r="C19" s="3" t="s">
         <v>110</v>
       </c>
@@ -1839,12 +2930,17 @@
       <c r="G19" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" ht="14" customHeight="1">
+      <c r="A20" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="8">
+        <v>2.1066666666666665</v>
+      </c>
       <c r="C20" s="3" t="s">
         <v>116</v>
       </c>
@@ -1870,11 +2966,13 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:10" ht="14" customHeight="1">
+      <c r="A21" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="8">
+        <v>2.8672000000000004</v>
+      </c>
       <c r="C21" s="3" t="s">
         <v>125</v>
       </c>
@@ -1890,12 +2988,17 @@
       <c r="G21" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="s">
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" ht="14" customHeight="1">
+      <c r="A22" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="8">
+        <v>1.5134693877551024</v>
+      </c>
       <c r="C22" s="3" t="s">
         <v>131</v>
       </c>
@@ -1917,12 +3020,15 @@
       <c r="I22" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" ht="13.75" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="8">
+        <v>2.7402439024390248</v>
+      </c>
       <c r="C23" s="3" t="s">
         <v>139</v>
       </c>
@@ -1941,12 +3047,16 @@
       <c r="H23" s="3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="s">
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" ht="14" customHeight="1">
+      <c r="A24" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="8">
+        <v>2.2328070175438599</v>
+      </c>
       <c r="C24" s="3" t="s">
         <v>146</v>
       </c>
@@ -1965,24 +3075,36 @@
       <c r="H24" s="3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="s">
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="14" customHeight="1">
+      <c r="A25" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="8">
+        <v>3.5756503642039541</v>
+      </c>
       <c r="C25" s="3" t="s">
         <v>153</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="s">
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" ht="14" customHeight="1">
+      <c r="A26" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="8">
+        <v>2.442535211267606</v>
+      </c>
       <c r="C26" s="3" t="s">
         <v>156</v>
       </c>
@@ -1992,24 +3114,39 @@
       <c r="E26" s="3" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="4" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" ht="14" customHeight="1">
+      <c r="A27" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="8">
+        <v>2.9598029556650247</v>
+      </c>
       <c r="C27" s="3" t="s">
         <v>160</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="4" t="s">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" ht="14" customHeight="1">
+      <c r="A28" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="8">
+        <v>2.2853448275862074</v>
+      </c>
       <c r="C28" s="3" t="s">
         <v>163</v>
       </c>
@@ -2019,36 +3156,59 @@
       <c r="E28" s="3" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" ht="13.75" customHeight="1">
+      <c r="A29" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="B29" s="7"/>
+      <c r="B29" s="8">
+        <v>1.8826229508196726</v>
+      </c>
       <c r="C29" s="3" t="s">
         <v>167</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="4" t="s">
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" ht="14" customHeight="1">
+      <c r="A30" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="8">
+        <v>0.73</v>
+      </c>
       <c r="C30" s="3" t="s">
         <v>170</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="4" t="s">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" ht="14" customHeight="1">
+      <c r="A31" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="8">
+        <v>2.9058959537572253</v>
+      </c>
       <c r="C31" s="3" t="s">
         <v>173</v>
       </c>
@@ -2058,12 +3218,19 @@
       <c r="E31" s="3" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="4" t="s">
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" ht="14" customHeight="1">
+      <c r="A32" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="8">
+        <v>2.5474509803921572</v>
+      </c>
       <c r="C32" s="3" t="s">
         <v>177</v>
       </c>
@@ -2073,12 +3240,19 @@
       <c r="E32" s="3" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="4" t="s">
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" ht="14" customHeight="1">
+      <c r="A33" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B33" s="7"/>
+      <c r="B33" s="8">
+        <v>0.55644444444444441</v>
+      </c>
       <c r="C33" s="3" t="s">
         <v>181</v>
       </c>
@@ -2088,24 +3262,39 @@
       <c r="E33" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="4" t="s">
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" ht="14" customHeight="1">
+      <c r="A34" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B34" s="7"/>
+      <c r="B34" s="8">
+        <v>1.0266666666666668</v>
+      </c>
       <c r="C34" s="3" t="s">
         <v>185</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="4" t="s">
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" ht="14" customHeight="1">
+      <c r="A35" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B35" s="7"/>
+      <c r="B35" s="8">
+        <v>0.11272727272727273</v>
+      </c>
       <c r="C35" s="3" t="s">
         <v>188</v>
       </c>
@@ -2115,12 +3304,19 @@
       <c r="E35" s="3" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="4" t="s">
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" ht="14" customHeight="1">
+      <c r="A36" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B36" s="7"/>
+      <c r="B36" s="8">
+        <v>2.5464285714285713</v>
+      </c>
       <c r="C36" s="3" t="s">
         <v>192</v>
       </c>
@@ -2130,36 +3326,59 @@
       <c r="E36" s="3" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="4" t="s">
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" ht="14" customHeight="1">
+      <c r="A37" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B37" s="7"/>
+      <c r="B37" s="8">
+        <v>1.475609756097561</v>
+      </c>
       <c r="C37" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="4" t="s">
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" ht="14" customHeight="1">
+      <c r="A38" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="B38" s="7"/>
+      <c r="B38" s="8">
+        <v>1.6243902439024389</v>
+      </c>
       <c r="C38" s="3" t="s">
         <v>199</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="4" t="s">
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" ht="14" customHeight="1">
+      <c r="A39" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B39" s="7"/>
+      <c r="B39" s="8">
+        <v>1.2928735632183908</v>
+      </c>
       <c r="C39" s="3" t="s">
         <v>202</v>
       </c>
@@ -2172,12 +3391,18 @@
       <c r="F39" s="3" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="4" t="s">
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:10" ht="14" customHeight="1">
+      <c r="A40" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B40" s="7"/>
+      <c r="B40" s="8">
+        <v>2.5035294117647058</v>
+      </c>
       <c r="C40" s="3" t="s">
         <v>207</v>
       </c>
@@ -2187,24 +3412,39 @@
       <c r="E40" s="3" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="4" t="s">
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:10" ht="14" customHeight="1">
+      <c r="A41" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B41" s="7"/>
+      <c r="B41" s="8">
+        <v>0.32909090909090905</v>
+      </c>
       <c r="C41" s="3" t="s">
         <v>211</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="4" t="s">
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:10" ht="14" customHeight="1">
+      <c r="A42" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B42" s="7"/>
+      <c r="B42" s="8">
+        <v>0.89999999999999991</v>
+      </c>
       <c r="C42" s="3" t="s">
         <v>214</v>
       </c>
@@ -2217,12 +3457,18 @@
       <c r="F42" s="3" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="4" t="s">
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="1:10" ht="14" customHeight="1">
+      <c r="A43" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B43" s="7"/>
+      <c r="B43" s="8">
+        <v>0.44285714285714284</v>
+      </c>
       <c r="C43" s="3" t="s">
         <v>219</v>
       </c>
@@ -2235,45 +3481,76 @@
       <c r="F43" s="3" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="4" t="s">
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="1:10" ht="14" customHeight="1">
+      <c r="A44" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B44" s="7"/>
+      <c r="B44" s="8">
+        <v>2.5825301204819278</v>
+      </c>
       <c r="C44" s="3" t="s">
         <v>224</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="1:10" ht="13.75" customHeight="1">
+      <c r="A45" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="B45" s="7"/>
+      <c r="B45" s="8">
+        <v>2.8544</v>
+      </c>
       <c r="C45" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="4" t="s">
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+    </row>
+    <row r="46" spans="1:10" ht="14" customHeight="1">
+      <c r="A46" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B46" s="7"/>
+      <c r="B46" s="8">
+        <v>2.9941935483870972</v>
+      </c>
       <c r="C46" s="3" t="s">
         <v>229</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="4" t="s">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+    </row>
+    <row r="47" spans="1:10" ht="14" customHeight="1">
+      <c r="A47" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B47" s="7"/>
+      <c r="B47" s="8">
+        <v>2.0723809523809527</v>
+      </c>
       <c r="C47" s="3" t="s">
         <v>232</v>
       </c>
@@ -2283,12 +3560,19 @@
       <c r="E47" s="3" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="4" t="s">
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+    </row>
+    <row r="48" spans="1:10" ht="14" customHeight="1">
+      <c r="A48" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B48" s="7"/>
+      <c r="B48" s="8">
+        <v>0.44571428571428573</v>
+      </c>
       <c r="C48" s="3" t="s">
         <v>236</v>
       </c>
@@ -2298,24 +3582,39 @@
       <c r="E48" s="3" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="4" t="s">
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+    </row>
+    <row r="49" spans="1:10" ht="14" customHeight="1">
+      <c r="A49" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="B49" s="7"/>
+      <c r="B49" s="8">
+        <v>2.2370833333333335</v>
+      </c>
       <c r="C49" s="3" t="s">
         <v>240</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="8" t="s">
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+    </row>
+    <row r="50" spans="1:10" ht="13.75" customHeight="1">
+      <c r="A50" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="B50" s="7"/>
+      <c r="B50" s="8">
+        <v>0</v>
+      </c>
       <c r="C50" s="3" t="s">
         <v>243</v>
       </c>
@@ -2328,24 +3627,38 @@
       <c r="F50" s="3" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="4" t="s">
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+    </row>
+    <row r="51" spans="1:10" ht="14" customHeight="1">
+      <c r="A51" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B51" s="7"/>
+      <c r="B51" s="8">
+        <v>0.90782608695652156</v>
+      </c>
       <c r="C51" s="3" t="s">
         <v>248</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="4" t="s">
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+    </row>
+    <row r="52" spans="1:10" ht="14" customHeight="1">
+      <c r="A52" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="B52" s="7"/>
+      <c r="B52" s="8">
+        <v>2.0438095238095242</v>
+      </c>
       <c r="C52" s="3" t="s">
         <v>251</v>
       </c>
@@ -2358,12 +3671,18 @@
       <c r="F52" s="3" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="4" t="s">
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+    </row>
+    <row r="53" spans="1:10" ht="14" customHeight="1">
+      <c r="A53" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="B53" s="9"/>
+      <c r="B53" s="8">
+        <v>2.7548603351955308</v>
+      </c>
       <c r="C53" s="3" t="s">
         <v>256</v>
       </c>
@@ -2373,12 +3692,19 @@
       <c r="E53" s="3" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="4" t="s">
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+    </row>
+    <row r="54" spans="1:10" ht="14" customHeight="1">
+      <c r="A54" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="B54" s="10"/>
+      <c r="B54" s="8">
+        <v>2.5886092715231785</v>
+      </c>
       <c r="C54" s="3" t="s">
         <v>260</v>
       </c>
@@ -2391,12 +3717,18 @@
       <c r="F54" s="3" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="4" t="s">
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+    </row>
+    <row r="55" spans="1:10" ht="14" customHeight="1">
+      <c r="A55" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="B55" s="10"/>
+      <c r="B55" s="8">
+        <v>1.8429906542056076</v>
+      </c>
       <c r="C55" s="3" t="s">
         <v>265</v>
       </c>
@@ -2412,12 +3744,17 @@
       <c r="G55" s="3" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="4" t="s">
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+    </row>
+    <row r="56" spans="1:10" ht="14" customHeight="1">
+      <c r="A56" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="B56" s="10"/>
+      <c r="B56" s="8">
+        <v>2.0354887218045117</v>
+      </c>
       <c r="C56" s="3" t="s">
         <v>271</v>
       </c>
@@ -2427,12 +3764,19 @@
       <c r="E56" s="3" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="4" t="s">
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+    </row>
+    <row r="57" spans="1:10" ht="14" customHeight="1">
+      <c r="A57" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B57" s="10"/>
+      <c r="B57" s="8">
+        <v>0.85142857142857153</v>
+      </c>
       <c r="C57" s="3" t="s">
         <v>275</v>
       </c>
@@ -2442,12 +3786,19 @@
       <c r="E57" s="3" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="4" t="s">
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+    </row>
+    <row r="58" spans="1:10" ht="14" customHeight="1">
+      <c r="A58" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="B58" s="10"/>
+      <c r="B58" s="8">
+        <v>1.1521621621621621</v>
+      </c>
       <c r="C58" s="3" t="s">
         <v>279</v>
       </c>
@@ -2457,48 +3808,79 @@
       <c r="E58" s="3" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="4" t="s">
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+    </row>
+    <row r="59" spans="1:10" ht="14" customHeight="1">
+      <c r="A59" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B59" s="10"/>
+      <c r="B59" s="8">
+        <v>1.3760000000000001</v>
+      </c>
       <c r="C59" s="3" t="s">
         <v>283</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="s">
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+    </row>
+    <row r="60" spans="1:10" ht="13.75" customHeight="1">
+      <c r="A60" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="B60" s="10"/>
+      <c r="B60" s="8">
+        <v>0.37200000000000005</v>
+      </c>
       <c r="C60" s="3" t="s">
         <v>286</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="s">
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+    </row>
+    <row r="61" spans="1:10" ht="13.75" customHeight="1">
+      <c r="A61" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="B61" s="10"/>
+      <c r="B61" s="8">
+        <v>2.8434285714285714</v>
+      </c>
       <c r="C61" s="3" t="s">
         <v>289</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="4" t="s">
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+    </row>
+    <row r="62" spans="1:10" ht="14" customHeight="1">
+      <c r="A62" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="B62" s="10"/>
+      <c r="B62" s="8">
+        <v>0.38062499999999999</v>
+      </c>
       <c r="C62" s="3" t="s">
         <v>292</v>
       </c>
@@ -2511,12 +3893,18 @@
       <c r="F62" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="4" t="s">
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+    </row>
+    <row r="63" spans="1:10" ht="14" customHeight="1">
+      <c r="A63" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="B63" s="10"/>
+      <c r="B63" s="8">
+        <v>1.6477064220183488</v>
+      </c>
       <c r="C63" s="3" t="s">
         <v>297</v>
       </c>
@@ -2526,12 +3914,19 @@
       <c r="E63" s="3" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="4" t="s">
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+    </row>
+    <row r="64" spans="1:10" ht="14" customHeight="1">
+      <c r="A64" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="B64" s="10"/>
+      <c r="B64" s="8">
+        <v>0.26181818181818178</v>
+      </c>
       <c r="C64" s="3" t="s">
         <v>301</v>
       </c>
@@ -2547,12 +3942,17 @@
       <c r="G64" s="3" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="4" t="s">
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+    </row>
+    <row r="65" spans="1:10" ht="14" customHeight="1">
+      <c r="A65" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="B65" s="10"/>
+      <c r="B65" s="8">
+        <v>3.0372571428571429</v>
+      </c>
       <c r="C65" s="3" t="s">
         <v>307</v>
       </c>
@@ -2562,12 +3962,19 @@
       <c r="E65" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="4" t="s">
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="1:10" ht="14" customHeight="1">
+      <c r="A66" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="B66" s="10"/>
+      <c r="B66" s="8">
+        <v>2.4059154929577473</v>
+      </c>
       <c r="C66" s="3" t="s">
         <v>311</v>
       </c>
@@ -2580,12 +3987,18 @@
       <c r="F66" s="3" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="4" t="s">
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+    </row>
+    <row r="67" spans="1:10" ht="14" customHeight="1">
+      <c r="A67" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="B67" s="10"/>
+      <c r="B67" s="8">
+        <v>0.71142857142857141</v>
+      </c>
       <c r="C67" s="3" t="s">
         <v>316</v>
       </c>
@@ -2595,12 +4008,19 @@
       <c r="E67" s="3" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="4" t="s">
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+    </row>
+    <row r="68" spans="1:10" ht="14" customHeight="1">
+      <c r="A68" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="B68" s="10"/>
+      <c r="B68" s="8">
+        <v>1.5079591836734698</v>
+      </c>
       <c r="C68" s="3" t="s">
         <v>320</v>
       </c>
@@ -2610,12 +4030,19 @@
       <c r="E68" s="3" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="4" t="s">
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+    </row>
+    <row r="69" spans="1:10" ht="14" customHeight="1">
+      <c r="A69" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="B69" s="10"/>
+      <c r="B69" s="8">
+        <v>2.592317880794702</v>
+      </c>
       <c r="C69" s="3" t="s">
         <v>324</v>
       </c>
@@ -2628,24 +4055,38 @@
       <c r="F69" s="3" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="4" t="s">
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+    </row>
+    <row r="70" spans="1:10" ht="14" customHeight="1">
+      <c r="A70" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="B70" s="10"/>
+      <c r="B70" s="8">
+        <v>2.5771428571428574</v>
+      </c>
       <c r="C70" s="3" t="s">
         <v>329</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="4" t="s">
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+    </row>
+    <row r="71" spans="1:10" ht="14" customHeight="1">
+      <c r="A71" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="B71" s="10"/>
+      <c r="B71" s="8">
+        <v>2.7987804878048781</v>
+      </c>
       <c r="C71" s="3" t="s">
         <v>332</v>
       </c>
@@ -2658,12 +4099,18 @@
       <c r="F71" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="4" t="s">
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+    </row>
+    <row r="72" spans="1:10" ht="14" customHeight="1">
+      <c r="A72" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="B72" s="10"/>
+      <c r="B72" s="8">
+        <v>1.2949999999999999</v>
+      </c>
       <c r="C72" s="3" t="s">
         <v>337</v>
       </c>
@@ -2676,24 +4123,38 @@
       <c r="F72" s="3" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="4" t="s">
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+    </row>
+    <row r="73" spans="1:10" ht="14" customHeight="1">
+      <c r="A73" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="B73" s="10"/>
+      <c r="B73" s="8">
+        <v>2.2995348837209302</v>
+      </c>
       <c r="C73" s="3" t="s">
         <v>342</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="4" t="s">
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+    </row>
+    <row r="74" spans="1:10" ht="14" customHeight="1">
+      <c r="A74" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="B74" s="10"/>
+      <c r="B74" s="8">
+        <v>2.1944067796610174</v>
+      </c>
       <c r="C74" s="3" t="s">
         <v>345</v>
       </c>
@@ -2703,33 +4164,57 @@
       <c r="E74" s="3" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="4" t="s">
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+    </row>
+    <row r="75" spans="1:10" ht="14" customHeight="1">
+      <c r="A75" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="B75" s="10"/>
+      <c r="B75" s="8">
+        <v>3.4377431906614784</v>
+      </c>
       <c r="C75" s="3" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="4" t="s">
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+    </row>
+    <row r="76" spans="1:10" ht="14" customHeight="1">
+      <c r="A76" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="B76" s="10"/>
+      <c r="B76" s="8">
+        <v>1.419795918367347</v>
+      </c>
       <c r="C76" s="3" t="s">
         <v>351</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="4" t="s">
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+    </row>
+    <row r="77" spans="1:10" ht="14" customHeight="1">
+      <c r="A77" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="B77" s="10"/>
+      <c r="B77" s="8">
+        <v>2.3447741935483872</v>
+      </c>
       <c r="C77" s="3" t="s">
         <v>354</v>
       </c>
@@ -2739,12 +4224,19 @@
       <c r="E77" s="3" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="4" t="s">
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+    </row>
+    <row r="78" spans="1:10" ht="14" customHeight="1">
+      <c r="A78" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="B78" s="10"/>
+      <c r="B78" s="8">
+        <v>0.66162162162162164</v>
+      </c>
       <c r="C78" s="3" t="s">
         <v>358</v>
       </c>
@@ -2754,9 +4246,18 @@
       <c r="E78" s="3" t="s">
         <v>360</v>
       </c>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>